<commit_message>
Merged records with activity #724
</commit_message>
<xml_diff>
--- a/scripts/RestClient/2ha/2ha_first_batch.xlsx
+++ b/scripts/RestClient/2ha/2ha_first_batch.xlsx
@@ -659,12 +659,6 @@
     <t>visibility</t>
   </si>
   <si>
-    <t>per_cover</t>
-  </si>
-  <si>
-    <t>undestorey_per_cover</t>
-  </si>
-  <si>
     <t>tracking_suitabliity</t>
   </si>
   <si>
@@ -789,6 +783,12 @@
   </si>
   <si>
     <t>percentOfPlotSuitable_4</t>
+  </si>
+  <si>
+    <t>percentCoverOverstorey</t>
+  </si>
+  <si>
+    <t>percentCoverUnderstorey</t>
   </si>
 </sst>
 </file>
@@ -898,7 +898,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="31">
+  <cellStyleXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -906,6 +906,32 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -970,7 +996,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="6"/>
   </cellXfs>
-  <cellStyles count="31">
+  <cellStyles count="57">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
@@ -985,6 +1011,19 @@
     <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
     <cellStyle name="Good" xfId="6" builtinId="26"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
@@ -1000,6 +1039,19 @@
     <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal_Sheet1" xfId="1"/>
   </cellStyles>
@@ -1286,7 +1338,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1296,8 +1348,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BG148"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AP1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="AP1" sqref="A1:XFD1"/>
+    <sheetView tabSelected="1" topLeftCell="Y1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="AG1" sqref="AG1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -1350,34 +1402,34 @@
   <sheetData>
     <row r="1" spans="1:59" s="17" customFormat="1" ht="15">
       <c r="A1" s="17" t="s">
+        <v>213</v>
+      </c>
+      <c r="B1" s="17" t="s">
+        <v>214</v>
+      </c>
+      <c r="C1" s="18" t="s">
+        <v>216</v>
+      </c>
+      <c r="D1" s="17" t="s">
         <v>215</v>
       </c>
-      <c r="B1" s="17" t="s">
-        <v>216</v>
-      </c>
-      <c r="C1" s="18" t="s">
-        <v>218</v>
-      </c>
-      <c r="D1" s="17" t="s">
+      <c r="E1" s="17" t="s">
         <v>217</v>
-      </c>
-      <c r="E1" s="17" t="s">
-        <v>219</v>
       </c>
       <c r="F1" s="17" t="s">
         <v>207</v>
       </c>
       <c r="G1" s="18" t="s">
+        <v>218</v>
+      </c>
+      <c r="H1" s="17" t="s">
+        <v>219</v>
+      </c>
+      <c r="I1" s="17" t="s">
         <v>220</v>
       </c>
-      <c r="H1" s="17" t="s">
+      <c r="J1" s="17" t="s">
         <v>221</v>
-      </c>
-      <c r="I1" s="17" t="s">
-        <v>222</v>
-      </c>
-      <c r="J1" s="17" t="s">
-        <v>223</v>
       </c>
       <c r="K1" s="17" t="s">
         <v>208</v>
@@ -1386,112 +1438,112 @@
         <v>209</v>
       </c>
       <c r="M1" s="20" t="s">
+        <v>222</v>
+      </c>
+      <c r="N1" s="18" t="s">
+        <v>223</v>
+      </c>
+      <c r="O1" s="18" t="s">
         <v>224</v>
       </c>
-      <c r="N1" s="18" t="s">
+      <c r="P1" s="18" t="s">
         <v>225</v>
       </c>
-      <c r="O1" s="18" t="s">
+      <c r="Q1" s="18" t="s">
         <v>226</v>
       </c>
-      <c r="P1" s="18" t="s">
+      <c r="R1" s="18" t="s">
         <v>227</v>
       </c>
-      <c r="Q1" s="18" t="s">
+      <c r="S1" s="18" t="s">
         <v>228</v>
       </c>
-      <c r="R1" s="18" t="s">
+      <c r="T1" s="18" t="s">
         <v>229</v>
-      </c>
-      <c r="S1" s="18" t="s">
-        <v>230</v>
-      </c>
-      <c r="T1" s="18" t="s">
-        <v>231</v>
       </c>
       <c r="U1" s="20" t="s">
         <v>210</v>
       </c>
       <c r="V1" s="18" t="s">
+        <v>230</v>
+      </c>
+      <c r="W1" s="18" t="s">
+        <v>231</v>
+      </c>
+      <c r="X1" s="18" t="s">
         <v>232</v>
       </c>
-      <c r="W1" s="18" t="s">
+      <c r="Y1" s="18" t="s">
         <v>233</v>
       </c>
-      <c r="X1" s="18" t="s">
+      <c r="Z1" s="18" t="s">
         <v>234</v>
       </c>
-      <c r="Y1" s="18" t="s">
+      <c r="AA1" s="18" t="s">
         <v>235</v>
       </c>
-      <c r="Z1" s="18" t="s">
+      <c r="AB1" s="20" t="s">
         <v>236</v>
       </c>
-      <c r="AA1" s="18" t="s">
+      <c r="AC1" s="20" t="s">
         <v>237</v>
       </c>
-      <c r="AB1" s="20" t="s">
+      <c r="AD1" s="20" t="s">
+        <v>253</v>
+      </c>
+      <c r="AE1" s="18" t="s">
         <v>238</v>
       </c>
-      <c r="AC1" s="20" t="s">
+      <c r="AF1" s="20" t="s">
         <v>239</v>
       </c>
-      <c r="AD1" s="19" t="s">
+      <c r="AG1" s="20" t="s">
+        <v>254</v>
+      </c>
+      <c r="AH1" s="20" t="s">
+        <v>249</v>
+      </c>
+      <c r="AI1" s="20" t="s">
+        <v>250</v>
+      </c>
+      <c r="AJ1" s="20" t="s">
+        <v>251</v>
+      </c>
+      <c r="AK1" s="18" t="s">
+        <v>252</v>
+      </c>
+      <c r="AL1" s="19" t="s">
         <v>211</v>
       </c>
-      <c r="AE1" s="18" t="s">
+      <c r="AM1" s="19" t="s">
+        <v>212</v>
+      </c>
+      <c r="AN1" s="20" t="s">
         <v>240</v>
       </c>
-      <c r="AF1" s="20" t="s">
+      <c r="AO1" s="20" t="s">
         <v>241</v>
       </c>
-      <c r="AG1" s="19" t="s">
-        <v>212</v>
-      </c>
-      <c r="AH1" s="20" t="s">
-        <v>251</v>
-      </c>
-      <c r="AI1" s="20" t="s">
-        <v>252</v>
-      </c>
-      <c r="AJ1" s="20" t="s">
-        <v>253</v>
-      </c>
-      <c r="AK1" s="18" t="s">
-        <v>254</v>
-      </c>
-      <c r="AL1" s="19" t="s">
-        <v>213</v>
-      </c>
-      <c r="AM1" s="19" t="s">
-        <v>214</v>
-      </c>
-      <c r="AN1" s="20" t="s">
+      <c r="AP1" s="20" t="s">
         <v>242</v>
       </c>
-      <c r="AO1" s="20" t="s">
+      <c r="AQ1" s="20" t="s">
         <v>243</v>
       </c>
-      <c r="AP1" s="20" t="s">
+      <c r="AR1" s="20" t="s">
         <v>244</v>
       </c>
-      <c r="AQ1" s="20" t="s">
+      <c r="AS1" s="20" t="s">
         <v>245</v>
       </c>
-      <c r="AR1" s="20" t="s">
+      <c r="AT1" s="20" t="s">
         <v>246</v>
       </c>
-      <c r="AS1" s="20" t="s">
+      <c r="AU1" s="20" t="s">
         <v>247</v>
       </c>
-      <c r="AT1" s="20" t="s">
+      <c r="AV1" s="20" t="s">
         <v>248</v>
-      </c>
-      <c r="AU1" s="20" t="s">
-        <v>249</v>
-      </c>
-      <c r="AV1" s="20" t="s">
-        <v>250</v>
       </c>
     </row>
     <row r="2" spans="1:59">

</xml_diff>